<commit_message>
fix bug level generator
</commit_message>
<xml_diff>
--- a/TankRunner/Assets/Resources/LD.xlsx
+++ b/TankRunner/Assets/Resources/LD.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12420"/>
+    <workbookView windowWidth="13305" windowHeight="4995"/>
   </bookViews>
   <sheets>
     <sheet name="elements" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="18">
   <si>
     <t>row</t>
   </si>
@@ -42,10 +42,13 @@
     <t>SideRight</t>
   </si>
   <si>
+    <t>T</t>
+  </si>
+  <si>
     <t>G</t>
   </si>
   <si>
-    <t>T</t>
+    <t>R</t>
   </si>
   <si>
     <t>H</t>
@@ -727,7 +730,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -748,6 +751,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1070,8 +1076,8 @@
   <sheetPr/>
   <dimension ref="A1:H118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G104" sqref="G104"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.90833333333333" defaultRowHeight="13.5" outlineLevelCol="7"/>
@@ -1187,9 +1193,24 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:7">
       <c r="A17" s="1">
         <v>16</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1197,7 +1218,7 @@
         <v>17</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1205,7 +1226,7 @@
         <v>18</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1213,7 +1234,7 @@
         <v>19</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1221,7 +1242,7 @@
         <v>20</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1229,12 +1250,18 @@
         <v>21</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="1">
         <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:1">
@@ -1247,7 +1274,7 @@
         <v>24</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1255,7 +1282,7 @@
         <v>25</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1263,20 +1290,26 @@
         <v>26</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" s="1">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1">
+      <c r="H28" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" s="1">
         <v>28</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1284,7 +1317,7 @@
         <v>29</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1292,7 +1325,7 @@
         <v>30</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1300,7 +1333,7 @@
         <v>31</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1308,7 +1341,7 @@
         <v>32</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1316,7 +1349,7 @@
         <v>33</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:1">
@@ -1329,7 +1362,7 @@
         <v>35</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1337,7 +1370,7 @@
         <v>36</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1345,7 +1378,7 @@
         <v>37</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1353,7 +1386,7 @@
         <v>38</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1361,7 +1394,7 @@
         <v>39</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:1">
@@ -1389,7 +1422,7 @@
         <v>44</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1397,7 +1430,7 @@
         <v>45</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1405,7 +1438,7 @@
         <v>46</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1413,7 +1446,7 @@
         <v>47</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1421,7 +1454,7 @@
         <v>48</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1429,7 +1462,7 @@
         <v>49</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:1">
@@ -1457,13 +1490,13 @@
         <v>54</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1471,7 +1504,7 @@
         <v>55</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1479,7 +1512,7 @@
         <v>56</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1487,7 +1520,7 @@
         <v>57</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:1">
@@ -1505,13 +1538,13 @@
         <v>60</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -1519,13 +1552,13 @@
         <v>61</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -1533,13 +1566,13 @@
         <v>62</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -1547,13 +1580,13 @@
         <v>63</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -1561,13 +1594,13 @@
         <v>64</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="66" spans="1:1">
@@ -1590,7 +1623,7 @@
         <v>68</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="70" spans="1:1">
@@ -1603,7 +1636,7 @@
         <v>70</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="72" spans="1:1">
@@ -1616,7 +1649,7 @@
         <v>72</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="74" spans="1:1">
@@ -1639,7 +1672,7 @@
         <v>76</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="78" spans="1:1">
@@ -1662,7 +1695,7 @@
         <v>80</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="82" spans="1:1">
@@ -1685,7 +1718,7 @@
         <v>84</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="86" spans="1:1">
@@ -1703,7 +1736,7 @@
         <v>87</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -1711,7 +1744,7 @@
         <v>88</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -1719,7 +1752,7 @@
         <v>89</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -1727,7 +1760,7 @@
         <v>90</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -1735,7 +1768,7 @@
         <v>91</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -1743,7 +1776,7 @@
         <v>92</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="94" spans="1:1">
@@ -1756,7 +1789,7 @@
         <v>94</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -1764,7 +1797,7 @@
         <v>95</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -1772,7 +1805,7 @@
         <v>96</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -1780,7 +1813,7 @@
         <v>97</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -1788,7 +1821,7 @@
         <v>98</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -1796,7 +1829,7 @@
         <v>99</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="101" spans="1:1">
@@ -1814,7 +1847,7 @@
         <v>102</v>
       </c>
       <c r="F103" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="104" spans="1:1">
@@ -1832,7 +1865,7 @@
         <v>105</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="107" spans="1:1">
@@ -1845,7 +1878,7 @@
         <v>107</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="109" spans="1:1">
@@ -1868,19 +1901,19 @@
         <v>111</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E112" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F112" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="113" spans="1:1">
@@ -1908,9 +1941,24 @@
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:1">
+    <row r="118" spans="1:7">
       <c r="A118" s="1">
         <v>117</v>
+      </c>
+      <c r="C118" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D118" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E118" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F118" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G118" s="7" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1933,175 +1981,175 @@
   <sheetData>
     <row r="18" spans="2:4">
       <c r="B18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="5:5">
       <c r="E22" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="4:4">
       <c r="D23" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="3:3">
       <c r="C24" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="3:3">
       <c r="C27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="3:3">
       <c r="C34" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="3:5">
       <c r="C37" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D37" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E37" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="3:3">
       <c r="C43" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="5:5">
       <c r="E44" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="5:5">
       <c r="E45" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="5:5">
       <c r="E46" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D49" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E49" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="53" spans="3:3">
       <c r="C53" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C55" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E55" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C56" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E56" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C57" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E57" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="58" spans="2:4">
       <c r="B58" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C58" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D58" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="3:3">
       <c r="C59" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="60" spans="2:4">
       <c r="B60" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D60" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E61" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="64" spans="3:3">
       <c r="C64" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2147,214 +2195,214 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D21" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="3:3">
       <c r="C26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="2:2">
       <c r="B29" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="3:3">
       <c r="C30" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="4:4">
       <c r="D31" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B32" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C32" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E32" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="4:4">
       <c r="D33" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="3:5">
       <c r="C34" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E34" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="4:4">
       <c r="D35" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="5:5">
       <c r="E36" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="2:4">
       <c r="B38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="3:5">
       <c r="C42" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D42" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E42" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="45" spans="3:3">
       <c r="C45" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="3:3">
       <c r="C46" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C47" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="3:3">
       <c r="C50" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="51" spans="3:3">
       <c r="C51" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52" spans="3:3">
       <c r="C52" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53" spans="3:3">
       <c r="C53" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="54" spans="4:4">
       <c r="D54" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="55" spans="3:3">
       <c r="C55" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="2:2">
       <c r="B56" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E57" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="59" spans="2:4">
       <c r="B59" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C59" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D59" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="66" spans="3:3">
       <c r="C66" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>